<commit_message>
minor changes to xlsx doc
</commit_message>
<xml_diff>
--- a/docs/ARM_Cortex_A9 32 Bit_dual_core.xlsx
+++ b/docs/ARM_Cortex_A9 32 Bit_dual_core.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
   <si>
     <t xml:space="preserve">Kalman Filter Sine Follower</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">AVG</t>
   </si>
   <si>
+    <t xml:space="preserve">32 bit processor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total</t>
   </si>
   <si>
@@ -68,11 +71,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -93,12 +97,6 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -153,7 +151,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,15 +172,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:O45"/>
+  <dimension ref="A2:Q45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36:O45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,6 +239,9 @@
       <c r="O6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="Q6" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -612,7 +613,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">SUM(B7:B14)</f>
@@ -639,7 +640,7 @@
         <v>7025.2</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J15" s="2" t="n">
         <f aca="false">SUM(J7:J14)</f>
@@ -668,7 +669,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,7 +1094,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">SUM(B22:B29)</f>
@@ -1120,7 +1121,7 @@
         <v>14803.2</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J30" s="2" t="n">
         <f aca="false">SUM(J22:J29)</f>
@@ -1149,7 +1150,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,7 +1575,7 @@
     </row>
     <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B45" s="0" t="n">
         <f aca="false">SUM(B37:B44)</f>
@@ -1601,7 +1602,7 @@
         <v>35024.8</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J45" s="2" t="n">
         <f aca="false">SUM(J37:J44)</f>

</xml_diff>